<commit_message>
Updated to have synchronization intead of just a .CheckExists for selecting the Transaction <Exec.Ref.> item.
</commit_message>
<xml_diff>
--- a/uft-one-ai-solman-start-tbom-recording/Default.xlsx
+++ b/uft-one-ai-solman-start-tbom-recording/Default.xlsx
@@ -548,8 +548,8 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>

</xml_diff>

<commit_message>
Updated because sometimes the ID column for filtering wouldn't display properly, used different navigation method to get to the ID filter.
</commit_message>
<xml_diff>
--- a/uft-one-ai-solman-start-tbom-recording/Default.xlsx
+++ b/uft-one-ai-solman-start-tbom-recording/Default.xlsx
@@ -31,9 +31,6 @@
     <t>https://sap-sm.mfdemoportal.com:50001/sap/bc/webdynpro/sap/smud_frame?sap-client=001&amp;sap-language=EN#</t>
   </si>
   <si>
-    <t>co03</t>
-  </si>
-  <si>
     <t>WorkItemNumber</t>
   </si>
   <si>
@@ -56,6 +53,9 @@
   </si>
   <si>
     <t>URL</t>
+  </si>
+  <si>
+    <t>co02</t>
   </si>
   <si>
     <t>https://sap-sm.mfdemoportal.com:50001/sap/bc/ui2/flp?sap-client=001&amp;sap-language=EN#Action-MyTasksBOM?VIEW_ID=TBWI&amp;STANDALONE_MODE=X</t>
@@ -549,7 +549,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -570,25 +570,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2">
@@ -602,10 +602,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F2" s="1">
         <v>302</v>

</xml_diff>